<commit_message>
Add Additional menu. Add time and date formats. Refactoring
</commit_message>
<xml_diff>
--- a/docs/eeprom.xlsx
+++ b/docs/eeprom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>Общая информация</t>
   </si>
@@ -95,15 +95,6 @@
     <t>byte</t>
   </si>
   <si>
-    <t>Системные настройки:</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>1 бит</t>
-  </si>
-  <si>
     <t>16…19</t>
   </si>
   <si>
@@ -125,115 +116,130 @@
     <t>Сохраненный текст на дисплее</t>
   </si>
   <si>
-    <t>80[0]</t>
-  </si>
-  <si>
-    <t>80[1]</t>
-  </si>
-  <si>
-    <t>80[2]</t>
-  </si>
-  <si>
-    <t>80[3]</t>
-  </si>
-  <si>
-    <t>80[4]</t>
-  </si>
-  <si>
-    <t>80[5]</t>
-  </si>
-  <si>
-    <t>80[6]</t>
-  </si>
-  <si>
-    <t>80[7]</t>
-  </si>
-  <si>
     <t>Страница 1</t>
   </si>
   <si>
-    <t>Разрешение на работу Канала 1</t>
-  </si>
-  <si>
-    <t>Разрешение на работу Канала 2</t>
-  </si>
-  <si>
-    <t>Разрешение на работу Канала 3</t>
-  </si>
-  <si>
-    <t>Разрешение на работу Канала 4</t>
-  </si>
-  <si>
-    <t>Разрешение на работу Канала 5</t>
-  </si>
-  <si>
-    <t>Разрешение на работу Канала 6</t>
-  </si>
-  <si>
-    <t>Разрешение на работу Канала 7</t>
-  </si>
-  <si>
-    <t>Разрешение на работу Канала 8</t>
-  </si>
-  <si>
     <t>Страница 0</t>
   </si>
   <si>
-    <t>81[0]</t>
-  </si>
-  <si>
-    <t>81[2]</t>
-  </si>
-  <si>
-    <t>81[1]</t>
-  </si>
-  <si>
-    <t>81[3]</t>
-  </si>
-  <si>
-    <t>81[4]</t>
-  </si>
-  <si>
-    <t>81[5]</t>
-  </si>
-  <si>
-    <t>81[6]</t>
-  </si>
-  <si>
-    <t>81[7]</t>
-  </si>
-  <si>
-    <t>Добавление Канала 1 на панель управления</t>
-  </si>
-  <si>
-    <t>Добавление Канала 2 на панель управления</t>
-  </si>
-  <si>
-    <t>Добавление Канала 3 на панель управления</t>
-  </si>
-  <si>
-    <t>Добавление Канала 4 на панель управления</t>
-  </si>
-  <si>
-    <t>Добавление Канала 5 на панель управления</t>
-  </si>
-  <si>
-    <t>Добавление Канала 6 на панель управления</t>
-  </si>
-  <si>
-    <t>Добавление Канала 7 на панель управления</t>
-  </si>
-  <si>
-    <t>Добавление Канала 8 на панель управления</t>
-  </si>
-  <si>
     <t>Период активации, с</t>
   </si>
   <si>
     <t>Длительность активации, с</t>
   </si>
   <si>
-    <t>1 Б</t>
+    <t>Добавление Канала N на панель управления</t>
+  </si>
+  <si>
+    <t>Разрешение на работу Канала N</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 Б
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>(1 бит * 8 каналов)</t>
+    </r>
+  </si>
+  <si>
+    <t>Настройка формата отображения времени:</t>
+  </si>
+  <si>
+    <t>Биты</t>
+  </si>
+  <si>
+    <t>0…7</t>
+  </si>
+  <si>
+    <t>0…1</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>чч:мм:сс</t>
+  </si>
+  <si>
+    <t>чч:мм</t>
+  </si>
+  <si>
+    <t>Настройка формата отображения даты:</t>
+  </si>
+  <si>
+    <t>ДД.ММ.ГГГГ</t>
+  </si>
+  <si>
+    <t>ДД.ММ.ГГ</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>3 бита</t>
+  </si>
+  <si>
+    <t>2…4</t>
+  </si>
+  <si>
+    <t>5…7</t>
+  </si>
+  <si>
+    <t>2 бит</t>
+  </si>
+  <si>
+    <t>ч:мм:сс</t>
+  </si>
+  <si>
+    <t>ч:мм</t>
+  </si>
+  <si>
+    <t>ДД-ММ-ГГГГ</t>
+  </si>
+  <si>
+    <t>ДД/ММ/ГГГГ</t>
+  </si>
+  <si>
+    <t>ММ-ДД-ГГГГ</t>
+  </si>
+  <si>
+    <t>ГГГГ-ММ-ДД</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -460,9 +466,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -490,6 +493,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -533,6 +545,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -854,489 +878,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="14.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+    <row r="1" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="4" t="s">
+    <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>80</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>81</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>82</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="38"/>
+      <c r="B13" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38"/>
+      <c r="B14" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38"/>
+      <c r="B15" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="38"/>
+      <c r="B16" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38"/>
+      <c r="B17" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38"/>
+      <c r="B18" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="39"/>
+    </row>
+    <row r="19" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38"/>
+      <c r="B19" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="39"/>
+    </row>
+    <row r="20" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="38"/>
+      <c r="B20" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="39"/>
+    </row>
+    <row r="21" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38"/>
+      <c r="B21" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="28"/>
+      <c r="E21" s="39"/>
+    </row>
+    <row r="22" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="38"/>
+      <c r="B22" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="39"/>
+    </row>
+    <row r="23" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="38"/>
+      <c r="B23" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="39"/>
+    </row>
+    <row r="24" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="38"/>
+      <c r="B24" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="28"/>
+      <c r="E24" s="39"/>
+    </row>
+    <row r="25" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="38"/>
+      <c r="B25" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="39"/>
+    </row>
+    <row r="26" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="38"/>
+      <c r="B26" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="C27" s="18"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+    </row>
+    <row r="30" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
+    </row>
+    <row r="31" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="B34" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
-        <v>81</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="19"/>
-    </row>
-    <row r="30" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="19"/>
-    </row>
-    <row r="31" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="19"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-    </row>
-    <row r="34" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="34"/>
-    </row>
-    <row r="35" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
-    </row>
-    <row r="36" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="4">
+    <row r="37" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="6">
+      <c r="D37" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="8">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C11:C18"/>
-    <mergeCell ref="A35:D35"/>
+  <mergeCells count="11">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="C20:C27"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A12:A26"/>
+    <mergeCell ref="D17:D25"/>
+    <mergeCell ref="E17:E25"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="E12:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B18:B21 B22:B25 B13:B16" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>